<commit_message>
Analise dos resultados do Ox
</commit_message>
<xml_diff>
--- a/Ox Metrics GVAR/Ox Scripts/Gvar_Determina WeakExo_v1_2020_11_13 (analise).xlsx
+++ b/Ox Metrics GVAR/Ox Scripts/Gvar_Determina WeakExo_v1_2020_11_13 (analise).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teo\Documents\Git\Tese\Ox Metrics GVAR\Ox Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bteba\Documents\GitHub\Tese\Ox Metrics GVAR\Ox Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4241CFAA-C22D-46F6-AA32-ADA2AAEB2894}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418EE82C-1DD6-4FE9-9405-FE9F7AAB1ADC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{947C9218-22C2-4F6D-A247-3378BCE994D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{947C9218-22C2-4F6D-A247-3378BCE994D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="9">
   <si>
     <t>Regiao</t>
   </si>
@@ -415,21 +415,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840D649B-3F87-4DA9-BA28-58A9BA50CAA6}">
   <dimension ref="A1:C556"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="R247" sqref="R247"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>0.01</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -440,7 +440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -451,7 +451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+1</f>
         <v>2</v>
@@ -463,7 +463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A68" si="0">A4+1</f>
         <v>3</v>
@@ -475,7 +475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -487,7 +487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -499,7 +499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -511,7 +511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -523,7 +523,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -535,7 +535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -547,7 +547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -559,7 +559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -571,7 +571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -583,7 +583,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -595,7 +595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -607,7 +607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -619,7 +619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -631,7 +631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -640,7 +640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -652,19 +652,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -676,7 +676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -688,7 +688,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -700,7 +700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -712,13 +712,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -730,7 +730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -742,7 +742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -754,7 +754,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -766,7 +766,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -778,7 +778,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -790,7 +790,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -802,7 +802,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -814,7 +814,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -826,7 +826,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -838,7 +838,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -850,7 +850,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -862,7 +862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -874,7 +874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -886,7 +886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -898,7 +898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -910,7 +910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -922,7 +922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -934,7 +934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -946,7 +946,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -958,7 +958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -970,7 +970,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -982,7 +982,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -994,7 +994,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1006,7 +1006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1018,7 +1018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -1030,7 +1030,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -1042,7 +1042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -1054,7 +1054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -1066,7 +1066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -1078,7 +1078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -1090,7 +1090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -1102,7 +1102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -1114,13 +1114,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -1132,7 +1132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -1144,7 +1144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -1156,7 +1156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -1168,7 +1168,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -1180,7 +1180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -1192,7 +1192,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -1204,7 +1204,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" ref="A69:A132" si="1">A68+1</f>
         <v>67</v>
@@ -1216,7 +1216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -1228,7 +1228,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -1240,7 +1240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -1252,7 +1252,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -1264,7 +1264,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -1276,7 +1276,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -1288,13 +1288,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -1306,7 +1306,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -1318,13 +1318,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -1336,7 +1336,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -1348,7 +1348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -1360,13 +1360,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -1378,7 +1378,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -1390,7 +1390,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -1402,7 +1402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -1414,7 +1414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -1426,7 +1426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -1438,7 +1438,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -1450,7 +1450,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -1462,7 +1462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -1474,7 +1474,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -1486,7 +1486,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -1498,7 +1498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -1510,7 +1510,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -1522,13 +1522,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -1540,7 +1540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -1552,7 +1552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -1564,7 +1564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -1576,7 +1576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -1588,2725 +1588,3439 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
+        <v>6</v>
+      </c>
+      <c r="C103" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>6</v>
+      </c>
+      <c r="C104" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
+        <v>6</v>
+      </c>
+      <c r="C105" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>3</v>
+      </c>
+      <c r="C106" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
+        <v>3</v>
+      </c>
+      <c r="C107" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
+        <v>6</v>
+      </c>
+      <c r="C108" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
+        <v>3</v>
+      </c>
+      <c r="C110" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <f t="shared" si="1"/>
         <v>109</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>3</v>
+      </c>
+      <c r="C111" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
+        <v>6</v>
+      </c>
+      <c r="C112" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <f t="shared" si="1"/>
         <v>111</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
+        <v>6</v>
+      </c>
+      <c r="C113" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B114" t="s">
+        <v>3</v>
+      </c>
+      <c r="C114" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
         <f t="shared" si="1"/>
         <v>113</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
+        <v>3</v>
+      </c>
+      <c r="C115" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
         <f t="shared" si="1"/>
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
+        <v>3</v>
+      </c>
+      <c r="C118" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B120" t="s">
+        <v>3</v>
+      </c>
+      <c r="C120" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
         <f t="shared" si="1"/>
         <v>119</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>3</v>
+      </c>
+      <c r="C121" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
+        <v>6</v>
+      </c>
+      <c r="C122" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
         <f t="shared" si="1"/>
         <v>121</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B123" t="s">
+        <v>3</v>
+      </c>
+      <c r="C123" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
         <f t="shared" si="1"/>
         <v>122</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B124" t="s">
+        <v>3</v>
+      </c>
+      <c r="C124" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
+        <v>3</v>
+      </c>
+      <c r="C125" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
+        <v>6</v>
+      </c>
+      <c r="C126" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
+        <v>3</v>
+      </c>
+      <c r="C127" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
         <f t="shared" si="1"/>
         <v>126</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B128" t="s">
+        <v>3</v>
+      </c>
+      <c r="C128" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B129" t="s">
+        <v>3</v>
+      </c>
+      <c r="C129" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B130" t="s">
+        <v>3</v>
+      </c>
+      <c r="C130" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131">
         <f t="shared" si="1"/>
         <v>129</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B131" t="s">
+        <v>6</v>
+      </c>
+      <c r="C131" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B132" t="s">
+        <v>3</v>
+      </c>
+      <c r="C132" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133">
         <f t="shared" ref="A133:A196" si="2">A132+1</f>
         <v>131</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B133" t="s">
+        <v>3</v>
+      </c>
+      <c r="C133" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
         <f t="shared" si="2"/>
         <v>132</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B134" t="s">
+        <v>3</v>
+      </c>
+      <c r="C134" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135">
         <f t="shared" si="2"/>
         <v>133</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
+        <v>3</v>
+      </c>
+      <c r="C135" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
         <f t="shared" si="2"/>
         <v>134</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
+        <v>3</v>
+      </c>
+      <c r="C136" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137">
         <f t="shared" si="2"/>
         <v>135</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
+        <v>3</v>
+      </c>
+      <c r="C137" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138">
         <f t="shared" si="2"/>
         <v>136</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
+        <v>6</v>
+      </c>
+      <c r="C138" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139">
         <f t="shared" si="2"/>
         <v>137</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B139" t="s">
+        <v>6</v>
+      </c>
+      <c r="C139" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140">
         <f t="shared" si="2"/>
         <v>138</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B140" t="s">
+        <v>6</v>
+      </c>
+      <c r="C140" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141">
         <f t="shared" si="2"/>
         <v>139</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B141" t="s">
+        <v>6</v>
+      </c>
+      <c r="C141" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142">
         <f t="shared" si="2"/>
         <v>140</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B142" t="s">
+        <v>3</v>
+      </c>
+      <c r="C142" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143">
         <f t="shared" si="2"/>
         <v>141</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B143" t="s">
+        <v>3</v>
+      </c>
+      <c r="C143" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144">
         <f t="shared" si="2"/>
         <v>142</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B144" t="s">
+        <v>6</v>
+      </c>
+      <c r="C144" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
         <f t="shared" si="2"/>
         <v>143</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B145" t="s">
+        <v>6</v>
+      </c>
+      <c r="C145" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
         <f t="shared" si="2"/>
         <v>144</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
         <f t="shared" si="2"/>
         <v>145</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B147" t="s">
+        <v>3</v>
+      </c>
+      <c r="C147" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
         <f t="shared" si="2"/>
         <v>146</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B148" t="s">
+        <v>6</v>
+      </c>
+      <c r="C148" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
         <f t="shared" si="2"/>
         <v>147</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B149" t="s">
+        <v>6</v>
+      </c>
+      <c r="C149" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
         <f t="shared" si="2"/>
         <v>148</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B150" t="s">
+        <v>6</v>
+      </c>
+      <c r="C150" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
         <f t="shared" si="2"/>
         <v>149</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B151" t="s">
+        <v>6</v>
+      </c>
+      <c r="C151" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B152" t="s">
+        <v>3</v>
+      </c>
+      <c r="C152" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153">
         <f t="shared" si="2"/>
         <v>151</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B153" t="s">
+        <v>3</v>
+      </c>
+      <c r="C153" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
         <f t="shared" si="2"/>
         <v>152</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B154" t="s">
+        <v>6</v>
+      </c>
+      <c r="C154" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
         <f t="shared" si="2"/>
         <v>153</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B155" t="s">
+        <v>3</v>
+      </c>
+      <c r="C155" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
         <f t="shared" si="2"/>
         <v>154</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B156" t="s">
+        <v>3</v>
+      </c>
+      <c r="C156" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
         <f t="shared" si="2"/>
         <v>155</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B157" t="s">
+        <v>3</v>
+      </c>
+      <c r="C157" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
         <f t="shared" si="2"/>
         <v>156</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B158" t="s">
+        <v>3</v>
+      </c>
+      <c r="C158" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
         <f t="shared" si="2"/>
         <v>157</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B159" t="s">
+        <v>3</v>
+      </c>
+      <c r="C159" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
         <f t="shared" si="2"/>
         <v>158</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B160" t="s">
+        <v>6</v>
+      </c>
+      <c r="C160" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161">
         <f t="shared" si="2"/>
         <v>159</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B161" t="s">
+        <v>6</v>
+      </c>
+      <c r="C161" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162">
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B162" t="s">
+        <v>6</v>
+      </c>
+      <c r="C162" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163">
         <f t="shared" si="2"/>
         <v>161</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B163" t="s">
+        <v>6</v>
+      </c>
+      <c r="C163" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164">
         <f t="shared" si="2"/>
         <v>162</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B164" t="s">
+        <v>6</v>
+      </c>
+      <c r="C164" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165">
         <f t="shared" si="2"/>
         <v>163</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B165" t="s">
+        <v>3</v>
+      </c>
+      <c r="C165" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166">
         <f t="shared" si="2"/>
         <v>164</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B166" t="s">
+        <v>3</v>
+      </c>
+      <c r="C166" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167">
         <f t="shared" si="2"/>
         <v>165</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B167" t="s">
+        <v>6</v>
+      </c>
+      <c r="C167" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168">
         <f t="shared" si="2"/>
         <v>166</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B168" t="s">
+        <v>6</v>
+      </c>
+      <c r="C168" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169">
         <f t="shared" si="2"/>
         <v>167</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B169" t="s">
+        <v>6</v>
+      </c>
+      <c r="C169" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170">
         <f t="shared" si="2"/>
         <v>168</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B170" t="s">
+        <v>6</v>
+      </c>
+      <c r="C170" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171">
         <f t="shared" si="2"/>
         <v>169</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B171" t="s">
+        <v>3</v>
+      </c>
+      <c r="C171" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172">
         <f t="shared" si="2"/>
         <v>170</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B172" t="s">
+        <v>3</v>
+      </c>
+      <c r="C172" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173">
         <f t="shared" si="2"/>
         <v>171</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B173" t="s">
+        <v>6</v>
+      </c>
+      <c r="C173" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174">
         <f t="shared" si="2"/>
         <v>172</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B174" t="s">
+        <v>3</v>
+      </c>
+      <c r="C174" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175">
         <f t="shared" si="2"/>
         <v>173</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B175" t="s">
+        <v>3</v>
+      </c>
+      <c r="C175" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176">
         <f t="shared" si="2"/>
         <v>174</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B176" t="s">
+        <v>6</v>
+      </c>
+      <c r="C176" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177">
         <f t="shared" si="2"/>
         <v>175</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B177" t="s">
+        <v>6</v>
+      </c>
+      <c r="C177" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178">
         <f t="shared" si="2"/>
         <v>176</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B178" t="s">
+        <v>6</v>
+      </c>
+      <c r="C178" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179">
         <f t="shared" si="2"/>
         <v>177</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B179" t="s">
+        <v>6</v>
+      </c>
+      <c r="C179" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180">
         <f t="shared" si="2"/>
         <v>178</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B180" t="s">
+        <v>6</v>
+      </c>
+      <c r="C180" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181">
         <f t="shared" si="2"/>
         <v>179</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B181" t="s">
+        <v>3</v>
+      </c>
+      <c r="C181" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B182" t="s">
+        <v>6</v>
+      </c>
+      <c r="C182" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183">
         <f t="shared" si="2"/>
         <v>181</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B183" t="s">
+        <v>6</v>
+      </c>
+      <c r="C183" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184">
         <f t="shared" si="2"/>
         <v>182</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B184" t="s">
+        <v>6</v>
+      </c>
+      <c r="C184" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185">
         <f t="shared" si="2"/>
         <v>183</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186">
         <f t="shared" si="2"/>
         <v>184</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187">
         <f t="shared" si="2"/>
         <v>185</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188">
         <f t="shared" si="2"/>
         <v>186</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B188" t="s">
+        <v>6</v>
+      </c>
+      <c r="C188" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189">
         <f t="shared" si="2"/>
         <v>187</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B189" t="s">
+        <v>6</v>
+      </c>
+      <c r="C189" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190">
         <f t="shared" si="2"/>
         <v>188</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B190" t="s">
+        <v>6</v>
+      </c>
+      <c r="C190" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191">
         <f t="shared" si="2"/>
         <v>189</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B191" t="s">
+        <v>3</v>
+      </c>
+      <c r="C191" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192">
         <f t="shared" si="2"/>
         <v>190</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B192" t="s">
+        <v>3</v>
+      </c>
+      <c r="C192" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193">
         <f t="shared" si="2"/>
         <v>191</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B193" t="s">
+        <v>6</v>
+      </c>
+      <c r="C193" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194">
         <f t="shared" si="2"/>
         <v>192</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B194" t="s">
+        <v>3</v>
+      </c>
+      <c r="C194" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195">
         <f t="shared" si="2"/>
         <v>193</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B195" t="s">
+        <v>6</v>
+      </c>
+      <c r="C195" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196">
         <f t="shared" si="2"/>
         <v>194</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B196" t="s">
+        <v>6</v>
+      </c>
+      <c r="C196" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197">
         <f t="shared" ref="A197:A260" si="3">A196+1</f>
         <v>195</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B197" t="s">
+        <v>6</v>
+      </c>
+      <c r="C197" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198">
         <f t="shared" si="3"/>
         <v>196</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B198" t="s">
+        <v>6</v>
+      </c>
+      <c r="C198" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199">
         <f t="shared" si="3"/>
         <v>197</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B199" t="s">
+        <v>3</v>
+      </c>
+      <c r="C199" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200">
         <f t="shared" si="3"/>
         <v>198</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B200" t="s">
+        <v>6</v>
+      </c>
+      <c r="C200" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201">
         <f t="shared" si="3"/>
         <v>199</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B201" t="s">
+        <v>6</v>
+      </c>
+      <c r="C201" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202">
         <f t="shared" si="3"/>
         <v>200</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B202" t="s">
+        <v>6</v>
+      </c>
+      <c r="C202" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203">
         <f t="shared" si="3"/>
         <v>201</v>
       </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B203" t="s">
+        <v>6</v>
+      </c>
+      <c r="C203" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204">
         <f t="shared" si="3"/>
         <v>202</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B204" t="s">
+        <v>3</v>
+      </c>
+      <c r="C204" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205">
         <f t="shared" si="3"/>
         <v>203</v>
       </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B205" t="s">
+        <v>6</v>
+      </c>
+      <c r="C205" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206">
         <f t="shared" si="3"/>
         <v>204</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B206" t="s">
+        <v>6</v>
+      </c>
+      <c r="C206" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207">
         <f t="shared" si="3"/>
         <v>205</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B207" t="s">
+        <v>6</v>
+      </c>
+      <c r="C207" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208">
         <f t="shared" si="3"/>
         <v>206</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B208" t="s">
+        <v>6</v>
+      </c>
+      <c r="C208" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209">
         <f t="shared" si="3"/>
         <v>207</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B209" t="s">
+        <v>6</v>
+      </c>
+      <c r="C209" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210">
         <f t="shared" si="3"/>
         <v>208</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B210" t="s">
+        <v>6</v>
+      </c>
+      <c r="C210" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211">
         <f t="shared" si="3"/>
         <v>209</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B211" t="s">
+        <v>6</v>
+      </c>
+      <c r="C211" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212">
         <f t="shared" si="3"/>
         <v>210</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B212" t="s">
+        <v>6</v>
+      </c>
+      <c r="C212" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213">
         <f t="shared" si="3"/>
         <v>211</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B213" t="s">
+        <v>6</v>
+      </c>
+      <c r="C213" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214">
         <f t="shared" si="3"/>
         <v>212</v>
       </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B214" t="s">
+        <v>3</v>
+      </c>
+      <c r="C214" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215">
         <f t="shared" si="3"/>
         <v>213</v>
       </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B215" t="s">
+        <v>3</v>
+      </c>
+      <c r="C215" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216">
         <f t="shared" si="3"/>
         <v>214</v>
       </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B216" t="s">
+        <v>6</v>
+      </c>
+      <c r="C216" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217">
         <f t="shared" si="3"/>
         <v>215</v>
       </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B217" t="s">
+        <v>6</v>
+      </c>
+      <c r="C217" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218">
         <f t="shared" si="3"/>
         <v>216</v>
       </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B218" t="s">
+        <v>6</v>
+      </c>
+      <c r="C218" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219">
         <f t="shared" si="3"/>
         <v>217</v>
       </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B219" t="s">
+        <v>6</v>
+      </c>
+      <c r="C219" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220">
         <f t="shared" si="3"/>
         <v>218</v>
       </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B220" t="s">
+        <v>6</v>
+      </c>
+      <c r="C220" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221">
         <f t="shared" si="3"/>
         <v>219</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B221" t="s">
+        <v>6</v>
+      </c>
+      <c r="C221" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222">
         <f t="shared" si="3"/>
         <v>220</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B222" t="s">
+        <v>3</v>
+      </c>
+      <c r="C222" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223">
         <f t="shared" si="3"/>
         <v>221</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224">
         <f t="shared" si="3"/>
         <v>222</v>
       </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B224" t="s">
+        <v>3</v>
+      </c>
+      <c r="C224" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225">
         <f t="shared" si="3"/>
         <v>223</v>
       </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B225" t="s">
+        <v>3</v>
+      </c>
+      <c r="C225" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226">
         <f t="shared" si="3"/>
         <v>224</v>
       </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B226" t="s">
+        <v>3</v>
+      </c>
+      <c r="C226" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227">
         <f t="shared" si="3"/>
         <v>225</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228">
         <f t="shared" si="3"/>
         <v>226</v>
       </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B228" t="s">
+        <v>6</v>
+      </c>
+      <c r="C228" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229">
         <f t="shared" si="3"/>
         <v>227</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230">
         <f t="shared" si="3"/>
         <v>228</v>
       </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B230" t="s">
+        <v>6</v>
+      </c>
+      <c r="C230" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231">
         <f t="shared" si="3"/>
         <v>229</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B231" t="s">
+        <v>3</v>
+      </c>
+      <c r="C231" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232">
         <f t="shared" si="3"/>
         <v>230</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233">
         <f t="shared" si="3"/>
         <v>231</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234">
         <f t="shared" si="3"/>
         <v>232</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235">
         <f t="shared" si="3"/>
         <v>233</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236">
         <f t="shared" si="3"/>
         <v>234</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237">
         <f t="shared" si="3"/>
         <v>235</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238">
         <f t="shared" si="3"/>
         <v>236</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239">
         <f t="shared" si="3"/>
         <v>237</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240">
         <f t="shared" si="3"/>
         <v>238</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241">
         <f t="shared" si="3"/>
         <v>239</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242">
         <f t="shared" si="3"/>
         <v>240</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243">
         <f t="shared" si="3"/>
         <v>241</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244">
         <f t="shared" si="3"/>
         <v>242</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245">
         <f t="shared" si="3"/>
         <v>243</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246">
         <f t="shared" si="3"/>
         <v>244</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247">
         <f t="shared" si="3"/>
         <v>245</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248">
         <f t="shared" si="3"/>
         <v>246</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249">
         <f t="shared" si="3"/>
         <v>247</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250">
         <f t="shared" si="3"/>
         <v>248</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251">
         <f t="shared" si="3"/>
         <v>249</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252">
         <f t="shared" si="3"/>
         <v>250</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253">
         <f t="shared" si="3"/>
         <v>251</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254">
         <f t="shared" si="3"/>
         <v>252</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255">
         <f t="shared" si="3"/>
         <v>253</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256">
         <f t="shared" si="3"/>
         <v>254</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257">
         <f t="shared" si="3"/>
         <v>255</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258">
         <f t="shared" si="3"/>
         <v>256</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259">
         <f t="shared" si="3"/>
         <v>257</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260">
         <f t="shared" si="3"/>
         <v>258</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261">
         <f t="shared" ref="A261:A324" si="4">A260+1</f>
         <v>259</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262">
         <f t="shared" si="4"/>
         <v>260</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263">
         <f t="shared" si="4"/>
         <v>261</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264">
         <f t="shared" si="4"/>
         <v>262</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265">
         <f t="shared" si="4"/>
         <v>263</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266">
         <f t="shared" si="4"/>
         <v>264</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267">
         <f t="shared" si="4"/>
         <v>265</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268">
         <f t="shared" si="4"/>
         <v>266</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269">
         <f t="shared" si="4"/>
         <v>267</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270">
         <f t="shared" si="4"/>
         <v>268</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271">
         <f t="shared" si="4"/>
         <v>269</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272">
         <f t="shared" si="4"/>
         <v>270</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273">
         <f t="shared" si="4"/>
         <v>271</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274">
         <f t="shared" si="4"/>
         <v>272</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275">
         <f t="shared" si="4"/>
         <v>273</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276">
         <f t="shared" si="4"/>
         <v>274</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277">
         <f t="shared" si="4"/>
         <v>275</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278">
         <f t="shared" si="4"/>
         <v>276</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279">
         <f t="shared" si="4"/>
         <v>277</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280">
         <f t="shared" si="4"/>
         <v>278</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281">
         <f t="shared" si="4"/>
         <v>279</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282">
         <f t="shared" si="4"/>
         <v>280</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283">
         <f t="shared" si="4"/>
         <v>281</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284">
         <f t="shared" si="4"/>
         <v>282</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285">
         <f t="shared" si="4"/>
         <v>283</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286">
         <f t="shared" si="4"/>
         <v>284</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287">
         <f t="shared" si="4"/>
         <v>285</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288">
         <f t="shared" si="4"/>
         <v>286</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289">
         <f t="shared" si="4"/>
         <v>287</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290">
         <f t="shared" si="4"/>
         <v>288</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291">
         <f t="shared" si="4"/>
         <v>289</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292">
         <f t="shared" si="4"/>
         <v>290</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293">
         <f t="shared" si="4"/>
         <v>291</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294">
         <f t="shared" si="4"/>
         <v>292</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295">
         <f t="shared" si="4"/>
         <v>293</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296">
         <f t="shared" si="4"/>
         <v>294</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297">
         <f t="shared" si="4"/>
         <v>295</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298">
         <f t="shared" si="4"/>
         <v>296</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299">
         <f t="shared" si="4"/>
         <v>297</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300">
         <f t="shared" si="4"/>
         <v>298</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301">
         <f t="shared" si="4"/>
         <v>299</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302">
         <f t="shared" si="4"/>
         <v>300</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303">
         <f t="shared" si="4"/>
         <v>301</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304">
         <f t="shared" si="4"/>
         <v>302</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305">
         <f t="shared" si="4"/>
         <v>303</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306">
         <f t="shared" si="4"/>
         <v>304</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307">
         <f t="shared" si="4"/>
         <v>305</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308">
         <f t="shared" si="4"/>
         <v>306</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A309">
         <f t="shared" si="4"/>
         <v>307</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310">
         <f t="shared" si="4"/>
         <v>308</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311">
         <f t="shared" si="4"/>
         <v>309</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A312">
         <f t="shared" si="4"/>
         <v>310</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313">
         <f t="shared" si="4"/>
         <v>311</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314">
         <f t="shared" si="4"/>
         <v>312</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315">
         <f t="shared" si="4"/>
         <v>313</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316">
         <f t="shared" si="4"/>
         <v>314</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317">
         <f t="shared" si="4"/>
         <v>315</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318">
         <f t="shared" si="4"/>
         <v>316</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319">
         <f t="shared" si="4"/>
         <v>317</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320">
         <f t="shared" si="4"/>
         <v>318</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321">
         <f t="shared" si="4"/>
         <v>319</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322">
         <f t="shared" si="4"/>
         <v>320</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323">
         <f t="shared" si="4"/>
         <v>321</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324">
         <f t="shared" si="4"/>
         <v>322</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325">
         <f t="shared" ref="A325:A388" si="5">A324+1</f>
         <v>323</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326">
         <f t="shared" si="5"/>
         <v>324</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A327">
         <f t="shared" si="5"/>
         <v>325</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328">
         <f t="shared" si="5"/>
         <v>326</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329">
         <f t="shared" si="5"/>
         <v>327</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A330">
         <f t="shared" si="5"/>
         <v>328</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331">
         <f t="shared" si="5"/>
         <v>329</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332">
         <f t="shared" si="5"/>
         <v>330</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333">
         <f t="shared" si="5"/>
         <v>331</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334">
         <f t="shared" si="5"/>
         <v>332</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335">
         <f t="shared" si="5"/>
         <v>333</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336">
         <f t="shared" si="5"/>
         <v>334</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337">
         <f t="shared" si="5"/>
         <v>335</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338">
         <f t="shared" si="5"/>
         <v>336</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339">
         <f t="shared" si="5"/>
         <v>337</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340">
         <f t="shared" si="5"/>
         <v>338</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341">
         <f t="shared" si="5"/>
         <v>339</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342">
         <f t="shared" si="5"/>
         <v>340</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343">
         <f t="shared" si="5"/>
         <v>341</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344">
         <f t="shared" si="5"/>
         <v>342</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A345">
         <f t="shared" si="5"/>
         <v>343</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346">
         <f t="shared" si="5"/>
         <v>344</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347">
         <f t="shared" si="5"/>
         <v>345</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A348">
         <f t="shared" si="5"/>
         <v>346</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349">
         <f t="shared" si="5"/>
         <v>347</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350">
         <f t="shared" si="5"/>
         <v>348</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A351">
         <f t="shared" si="5"/>
         <v>349</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352">
         <f t="shared" si="5"/>
         <v>350</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353">
         <f t="shared" si="5"/>
         <v>351</v>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A354">
         <f t="shared" si="5"/>
         <v>352</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355">
         <f t="shared" si="5"/>
         <v>353</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356">
         <f t="shared" si="5"/>
         <v>354</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357">
         <f t="shared" si="5"/>
         <v>355</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358">
         <f t="shared" si="5"/>
         <v>356</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359">
         <f t="shared" si="5"/>
         <v>357</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360">
         <f t="shared" si="5"/>
         <v>358</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361">
         <f t="shared" si="5"/>
         <v>359</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362">
         <f t="shared" si="5"/>
         <v>360</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363">
         <f t="shared" si="5"/>
         <v>361</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364">
         <f t="shared" si="5"/>
         <v>362</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365">
         <f t="shared" si="5"/>
         <v>363</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A366">
         <f t="shared" si="5"/>
         <v>364</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367">
         <f t="shared" si="5"/>
         <v>365</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368">
         <f t="shared" si="5"/>
         <v>366</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A369">
         <f t="shared" si="5"/>
         <v>367</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370">
         <f t="shared" si="5"/>
         <v>368</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371">
         <f t="shared" si="5"/>
         <v>369</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A372">
         <f t="shared" si="5"/>
         <v>370</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373">
         <f t="shared" si="5"/>
         <v>371</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374">
         <f t="shared" si="5"/>
         <v>372</v>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375">
         <f t="shared" si="5"/>
         <v>373</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376">
         <f t="shared" si="5"/>
         <v>374</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377">
         <f t="shared" si="5"/>
         <v>375</v>
       </c>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378">
         <f t="shared" si="5"/>
         <v>376</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379">
         <f t="shared" si="5"/>
         <v>377</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380">
         <f t="shared" si="5"/>
         <v>378</v>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381">
         <f t="shared" si="5"/>
         <v>379</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382">
         <f t="shared" si="5"/>
         <v>380</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383">
         <f t="shared" si="5"/>
         <v>381</v>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A384">
         <f t="shared" si="5"/>
         <v>382</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385">
         <f t="shared" si="5"/>
         <v>383</v>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386">
         <f t="shared" si="5"/>
         <v>384</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A387">
         <f t="shared" si="5"/>
         <v>385</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A388">
         <f t="shared" si="5"/>
         <v>386</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A389">
         <f t="shared" ref="A389:A452" si="6">A388+1</f>
         <v>387</v>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A390">
         <f t="shared" si="6"/>
         <v>388</v>
       </c>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391">
         <f t="shared" si="6"/>
         <v>389</v>
       </c>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392">
         <f t="shared" si="6"/>
         <v>390</v>
       </c>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393">
         <f t="shared" si="6"/>
         <v>391</v>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394">
         <f t="shared" si="6"/>
         <v>392</v>
       </c>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395">
         <f t="shared" si="6"/>
         <v>393</v>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396">
         <f t="shared" si="6"/>
         <v>394</v>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397">
         <f t="shared" si="6"/>
         <v>395</v>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398">
         <f t="shared" si="6"/>
         <v>396</v>
       </c>
     </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399">
         <f t="shared" si="6"/>
         <v>397</v>
       </c>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400">
         <f t="shared" si="6"/>
         <v>398</v>
       </c>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401">
         <f t="shared" si="6"/>
         <v>399</v>
       </c>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A402">
         <f t="shared" si="6"/>
         <v>400</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A403">
         <f t="shared" si="6"/>
         <v>401</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404">
         <f t="shared" si="6"/>
         <v>402</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A405">
         <f t="shared" si="6"/>
         <v>403</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406">
         <f t="shared" si="6"/>
         <v>404</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A407">
         <f t="shared" si="6"/>
         <v>405</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A408">
         <f t="shared" si="6"/>
         <v>406</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409">
         <f t="shared" si="6"/>
         <v>407</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A410">
         <f t="shared" si="6"/>
         <v>408</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A411">
         <f t="shared" si="6"/>
         <v>409</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A412">
         <f t="shared" si="6"/>
         <v>410</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A413">
         <f t="shared" si="6"/>
         <v>411</v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A414">
         <f t="shared" si="6"/>
         <v>412</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A415">
         <f t="shared" si="6"/>
         <v>413</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A416">
         <f t="shared" si="6"/>
         <v>414</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A417">
         <f t="shared" si="6"/>
         <v>415</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418">
         <f t="shared" si="6"/>
         <v>416</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A419">
         <f t="shared" si="6"/>
         <v>417</v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A420">
         <f t="shared" si="6"/>
         <v>418</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A421">
         <f t="shared" si="6"/>
         <v>419</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A422">
         <f t="shared" si="6"/>
         <v>420</v>
       </c>
     </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A423">
         <f t="shared" si="6"/>
         <v>421</v>
       </c>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A424">
         <f t="shared" si="6"/>
         <v>422</v>
       </c>
     </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A425">
         <f t="shared" si="6"/>
         <v>423</v>
       </c>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A426">
         <f t="shared" si="6"/>
         <v>424</v>
       </c>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A427">
         <f t="shared" si="6"/>
         <v>425</v>
       </c>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A428">
         <f t="shared" si="6"/>
         <v>426</v>
       </c>
     </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A429">
         <f t="shared" si="6"/>
         <v>427</v>
       </c>
     </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A430">
         <f t="shared" si="6"/>
         <v>428</v>
       </c>
     </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A431">
         <f t="shared" si="6"/>
         <v>429</v>
       </c>
     </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A432">
         <f t="shared" si="6"/>
         <v>430</v>
       </c>
     </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433">
         <f t="shared" si="6"/>
         <v>431</v>
       </c>
     </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434">
         <f t="shared" si="6"/>
         <v>432</v>
       </c>
     </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A435">
         <f t="shared" si="6"/>
         <v>433</v>
       </c>
     </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436">
         <f t="shared" si="6"/>
         <v>434</v>
       </c>
     </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437">
         <f t="shared" si="6"/>
         <v>435</v>
       </c>
     </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A438">
         <f t="shared" si="6"/>
         <v>436</v>
       </c>
     </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439">
         <f t="shared" si="6"/>
         <v>437</v>
       </c>
     </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A440">
         <f t="shared" si="6"/>
         <v>438</v>
       </c>
     </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A441">
         <f t="shared" si="6"/>
         <v>439</v>
       </c>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A442">
         <f t="shared" si="6"/>
         <v>440</v>
       </c>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A443">
         <f t="shared" si="6"/>
         <v>441</v>
       </c>
     </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A444">
         <f t="shared" si="6"/>
         <v>442</v>
       </c>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A445">
         <f t="shared" si="6"/>
         <v>443</v>
       </c>
     </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A446">
         <f t="shared" si="6"/>
         <v>444</v>
       </c>
     </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A447">
         <f t="shared" si="6"/>
         <v>445</v>
       </c>
     </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A448">
         <f t="shared" si="6"/>
         <v>446</v>
       </c>
     </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A449">
         <f t="shared" si="6"/>
         <v>447</v>
       </c>
     </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A450">
         <f t="shared" si="6"/>
         <v>448</v>
       </c>
     </row>
-    <row r="451" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A451">
         <f t="shared" si="6"/>
         <v>449</v>
       </c>
     </row>
-    <row r="452" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A452">
         <f t="shared" si="6"/>
         <v>450</v>
       </c>
     </row>
-    <row r="453" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A453">
         <f t="shared" ref="A453:A516" si="7">A452+1</f>
         <v>451</v>
       </c>
     </row>
-    <row r="454" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A454">
         <f t="shared" si="7"/>
         <v>452</v>
       </c>
     </row>
-    <row r="455" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455">
         <f t="shared" si="7"/>
         <v>453</v>
       </c>
     </row>
-    <row r="456" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A456">
         <f t="shared" si="7"/>
         <v>454</v>
       </c>
     </row>
-    <row r="457" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A457">
         <f t="shared" si="7"/>
         <v>455</v>
       </c>
     </row>
-    <row r="458" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A458">
         <f t="shared" si="7"/>
         <v>456</v>
       </c>
     </row>
-    <row r="459" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A459">
         <f t="shared" si="7"/>
         <v>457</v>
       </c>
     </row>
-    <row r="460" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A460">
         <f t="shared" si="7"/>
         <v>458</v>
       </c>
     </row>
-    <row r="461" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461">
         <f t="shared" si="7"/>
         <v>459</v>
       </c>
     </row>
-    <row r="462" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A462">
         <f t="shared" si="7"/>
         <v>460</v>
       </c>
     </row>
-    <row r="463" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A463">
         <f t="shared" si="7"/>
         <v>461</v>
       </c>
     </row>
-    <row r="464" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A464">
         <f t="shared" si="7"/>
         <v>462</v>
       </c>
     </row>
-    <row r="465" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A465">
         <f t="shared" si="7"/>
         <v>463</v>
       </c>
     </row>
-    <row r="466" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A466">
         <f t="shared" si="7"/>
         <v>464</v>
       </c>
     </row>
-    <row r="467" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A467">
         <f t="shared" si="7"/>
         <v>465</v>
       </c>
     </row>
-    <row r="468" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A468">
         <f t="shared" si="7"/>
         <v>466</v>
       </c>
     </row>
-    <row r="469" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A469">
         <f t="shared" si="7"/>
         <v>467</v>
       </c>
     </row>
-    <row r="470" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A470">
         <f t="shared" si="7"/>
         <v>468</v>
       </c>
     </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A471">
         <f t="shared" si="7"/>
         <v>469</v>
       </c>
     </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A472">
         <f t="shared" si="7"/>
         <v>470</v>
       </c>
     </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A473">
         <f t="shared" si="7"/>
         <v>471</v>
       </c>
     </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A474">
         <f t="shared" si="7"/>
         <v>472</v>
       </c>
     </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A475">
         <f t="shared" si="7"/>
         <v>473</v>
       </c>
     </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A476">
         <f t="shared" si="7"/>
         <v>474</v>
       </c>
     </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A477">
         <f t="shared" si="7"/>
         <v>475</v>
       </c>
     </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A478">
         <f t="shared" si="7"/>
         <v>476</v>
       </c>
     </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A479">
         <f t="shared" si="7"/>
         <v>477</v>
       </c>
     </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A480">
         <f t="shared" si="7"/>
         <v>478</v>
       </c>
     </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A481">
         <f t="shared" si="7"/>
         <v>479</v>
       </c>
     </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A482">
         <f t="shared" si="7"/>
         <v>480</v>
       </c>
     </row>
-    <row r="483" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A483">
         <f t="shared" si="7"/>
         <v>481</v>
       </c>
     </row>
-    <row r="484" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A484">
         <f t="shared" si="7"/>
         <v>482</v>
       </c>
     </row>
-    <row r="485" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A485">
         <f t="shared" si="7"/>
         <v>483</v>
       </c>
     </row>
-    <row r="486" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A486">
         <f t="shared" si="7"/>
         <v>484</v>
       </c>
     </row>
-    <row r="487" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A487">
         <f t="shared" si="7"/>
         <v>485</v>
       </c>
     </row>
-    <row r="488" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A488">
         <f t="shared" si="7"/>
         <v>486</v>
       </c>
     </row>
-    <row r="489" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A489">
         <f t="shared" si="7"/>
         <v>487</v>
       </c>
     </row>
-    <row r="490" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A490">
         <f t="shared" si="7"/>
         <v>488</v>
       </c>
     </row>
-    <row r="491" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A491">
         <f t="shared" si="7"/>
         <v>489</v>
       </c>
     </row>
-    <row r="492" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492">
         <f t="shared" si="7"/>
         <v>490</v>
       </c>
     </row>
-    <row r="493" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A493">
         <f t="shared" si="7"/>
         <v>491</v>
       </c>
     </row>
-    <row r="494" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A494">
         <f t="shared" si="7"/>
         <v>492</v>
       </c>
     </row>
-    <row r="495" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A495">
         <f t="shared" si="7"/>
         <v>493</v>
       </c>
     </row>
-    <row r="496" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A496">
         <f t="shared" si="7"/>
         <v>494</v>
       </c>
     </row>
-    <row r="497" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A497">
         <f t="shared" si="7"/>
         <v>495</v>
       </c>
     </row>
-    <row r="498" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A498">
         <f t="shared" si="7"/>
         <v>496</v>
       </c>
     </row>
-    <row r="499" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A499">
         <f t="shared" si="7"/>
         <v>497</v>
       </c>
     </row>
-    <row r="500" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A500">
         <f t="shared" si="7"/>
         <v>498</v>
       </c>
     </row>
-    <row r="501" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A501">
         <f t="shared" si="7"/>
         <v>499</v>
       </c>
     </row>
-    <row r="502" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A502">
         <f t="shared" si="7"/>
         <v>500</v>
       </c>
     </row>
-    <row r="503" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A503">
         <f t="shared" si="7"/>
         <v>501</v>
       </c>
     </row>
-    <row r="504" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A504">
         <f t="shared" si="7"/>
         <v>502</v>
       </c>
     </row>
-    <row r="505" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A505">
         <f t="shared" si="7"/>
         <v>503</v>
       </c>
     </row>
-    <row r="506" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A506">
         <f t="shared" si="7"/>
         <v>504</v>
       </c>
     </row>
-    <row r="507" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A507">
         <f t="shared" si="7"/>
         <v>505</v>
       </c>
     </row>
-    <row r="508" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A508">
         <f t="shared" si="7"/>
         <v>506</v>
       </c>
     </row>
-    <row r="509" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A509">
         <f t="shared" si="7"/>
         <v>507</v>
       </c>
     </row>
-    <row r="510" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A510">
         <f t="shared" si="7"/>
         <v>508</v>
       </c>
     </row>
-    <row r="511" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A511">
         <f t="shared" si="7"/>
         <v>509</v>
       </c>
     </row>
-    <row r="512" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A512">
         <f t="shared" si="7"/>
         <v>510</v>
       </c>
     </row>
-    <row r="513" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A513">
         <f t="shared" si="7"/>
         <v>511</v>
       </c>
     </row>
-    <row r="514" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A514">
         <f t="shared" si="7"/>
         <v>512</v>
       </c>
     </row>
-    <row r="515" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A515">
         <f t="shared" si="7"/>
         <v>513</v>
       </c>
     </row>
-    <row r="516" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A516">
         <f t="shared" si="7"/>
         <v>514</v>
       </c>
     </row>
-    <row r="517" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A517">
         <f t="shared" ref="A517:A556" si="8">A516+1</f>
         <v>515</v>
       </c>
     </row>
-    <row r="518" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A518">
         <f t="shared" si="8"/>
         <v>516</v>
       </c>
     </row>
-    <row r="519" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A519">
         <f t="shared" si="8"/>
         <v>517</v>
       </c>
     </row>
-    <row r="520" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A520">
         <f t="shared" si="8"/>
         <v>518</v>
       </c>
     </row>
-    <row r="521" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A521">
         <f t="shared" si="8"/>
         <v>519</v>
       </c>
     </row>
-    <row r="522" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A522">
         <f t="shared" si="8"/>
         <v>520</v>
       </c>
     </row>
-    <row r="523" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A523">
         <f t="shared" si="8"/>
         <v>521</v>
       </c>
     </row>
-    <row r="524" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A524">
         <f t="shared" si="8"/>
         <v>522</v>
       </c>
     </row>
-    <row r="525" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A525">
         <f t="shared" si="8"/>
         <v>523</v>
       </c>
     </row>
-    <row r="526" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A526">
         <f t="shared" si="8"/>
         <v>524</v>
       </c>
     </row>
-    <row r="527" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A527">
         <f t="shared" si="8"/>
         <v>525</v>
       </c>
     </row>
-    <row r="528" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A528">
         <f t="shared" si="8"/>
         <v>526</v>
       </c>
     </row>
-    <row r="529" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A529">
         <f t="shared" si="8"/>
         <v>527</v>
       </c>
     </row>
-    <row r="530" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A530">
         <f t="shared" si="8"/>
         <v>528</v>
       </c>
     </row>
-    <row r="531" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A531">
         <f t="shared" si="8"/>
         <v>529</v>
       </c>
     </row>
-    <row r="532" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A532">
         <f t="shared" si="8"/>
         <v>530</v>
       </c>
     </row>
-    <row r="533" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A533">
         <f t="shared" si="8"/>
         <v>531</v>
       </c>
     </row>
-    <row r="534" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A534">
         <f t="shared" si="8"/>
         <v>532</v>
       </c>
     </row>
-    <row r="535" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A535">
         <f t="shared" si="8"/>
         <v>533</v>
       </c>
     </row>
-    <row r="536" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A536">
         <f t="shared" si="8"/>
         <v>534</v>
       </c>
     </row>
-    <row r="537" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A537">
         <f t="shared" si="8"/>
         <v>535</v>
       </c>
     </row>
-    <row r="538" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A538">
         <f t="shared" si="8"/>
         <v>536</v>
       </c>
     </row>
-    <row r="539" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A539">
         <f t="shared" si="8"/>
         <v>537</v>
       </c>
     </row>
-    <row r="540" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A540">
         <f t="shared" si="8"/>
         <v>538</v>
       </c>
     </row>
-    <row r="541" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A541">
         <f t="shared" si="8"/>
         <v>539</v>
       </c>
     </row>
-    <row r="542" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A542">
         <f t="shared" si="8"/>
         <v>540</v>
       </c>
     </row>
-    <row r="543" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A543">
         <f t="shared" si="8"/>
         <v>541</v>
       </c>
     </row>
-    <row r="544" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A544">
         <f t="shared" si="8"/>
         <v>542</v>
       </c>
     </row>
-    <row r="545" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A545">
         <f t="shared" si="8"/>
         <v>543</v>
       </c>
     </row>
-    <row r="546" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A546">
         <f t="shared" si="8"/>
         <v>544</v>
       </c>
     </row>
-    <row r="547" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A547">
         <f t="shared" si="8"/>
         <v>545</v>
       </c>
     </row>
-    <row r="548" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A548">
         <f t="shared" si="8"/>
         <v>546</v>
       </c>
     </row>
-    <row r="549" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A549">
         <f t="shared" si="8"/>
         <v>547</v>
       </c>
     </row>
-    <row r="550" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A550">
         <f t="shared" si="8"/>
         <v>548</v>
       </c>
     </row>
-    <row r="551" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A551">
         <f t="shared" si="8"/>
         <v>549</v>
       </c>
     </row>
-    <row r="552" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A552">
         <f t="shared" si="8"/>
         <v>550</v>
       </c>
     </row>
-    <row r="553" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A553">
         <f t="shared" si="8"/>
         <v>551</v>
       </c>
     </row>
-    <row r="554" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A554">
         <f t="shared" si="8"/>
         <v>552</v>
       </c>
     </row>
-    <row r="555" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A555">
         <f t="shared" si="8"/>
         <v>553</v>
       </c>
     </row>
-    <row r="556" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A556">
         <f t="shared" si="8"/>
         <v>554</v>

</xml_diff>